<commit_message>
added files & changes somes files
</commit_message>
<xml_diff>
--- a/Sheet/FINAL450.xlsx
+++ b/Sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS &amp; ALGO\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCBD77C-F95F-489D-9DDA-8E154B44FC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC211B33-A03F-4F72-AE92-1E676CE85C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -2014,8 +2014,8 @@
       <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>4</v>
+      <c r="C13" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -5269,8 +5269,8 @@
       <c r="B321" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C321" s="4" t="s">
-        <v>4</v>
+      <c r="C321" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added more tree files
</commit_message>
<xml_diff>
--- a/Sheet/FINAL450.xlsx
+++ b/Sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS &amp; ALGO\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EA32C2-D2F8-4CDC-9A3D-2D8778CCFFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299D925F-6F90-4991-8767-243D9A00076A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3766,8 +3766,8 @@
       <c r="B180" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C180" s="4" t="s">
-        <v>4</v>
+      <c r="C180" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3777,8 +3777,8 @@
       <c r="B181" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C181" s="4" t="s">
-        <v>4</v>
+      <c r="C181" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added sorting searcing file & tree files
</commit_message>
<xml_diff>
--- a/Sheet/FINAL450.xlsx
+++ b/Sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS &amp; ALGO\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309324CD-9CFB-474E-ABB8-A7FA1D0A3577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D7028E-C387-4283-A9E4-99734A1D0BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1899,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -2954,8 +2954,8 @@
       <c r="B102" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>4</v>
+      <c r="C102" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -2987,8 +2987,8 @@
       <c r="B105" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C105" s="4" t="s">
-        <v>4</v>
+      <c r="C105" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="21">
@@ -3917,8 +3917,8 @@
       <c r="B192" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C192" s="4" t="s">
-        <v>4</v>
+      <c r="C192" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added searching sorting file
</commit_message>
<xml_diff>
--- a/Sheet/FINAL450.xlsx
+++ b/Sheet/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS &amp; ALGO\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D7028E-C387-4283-A9E4-99734A1D0BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B83DC7D-879F-4C86-A972-3D7CF579C29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1899,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
@@ -3075,8 +3075,8 @@
       <c r="B113" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>4</v>
+      <c r="C113" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="21">

</xml_diff>